<commit_message>
creating test cases related to User Story 4
</commit_message>
<xml_diff>
--- a/TestCases/UserStory4.xlsx
+++ b/TestCases/UserStory4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ParaBank\web-application-testing\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2E587A-22BA-42DC-AC8C-7B9BBD873BF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209B127F-67FA-4AD8-AFC7-89ED0399D95E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="869" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="869" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User selects account type " sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>TC_USAT_001</t>
-  </si>
-  <si>
-    <t>Verify User can select account Type (Checking, Saving)</t>
   </si>
   <si>
     <t>1. user open the website (https://parabank.parasoft.com/parabank/index.htm)
@@ -101,6 +98,110 @@
     <t xml:space="preserve">Account Opened!
 Congratulations, your account is now open.
 Your new account number: xxxxx
+</t>
+  </si>
+  <si>
+    <t>TC_USAT_002</t>
+  </si>
+  <si>
+    <t>Verify User cannot create account using insuffecient balance in another account.</t>
+  </si>
+  <si>
+    <t>1. user open the website (https://parabank.parasoft.com/parabank/index.htm)
+2.Login using username &amp; password.
+3. Choose Open new account from the side menu bar.
+4. select account type from the menu (saving, checking)
+5.choose the account number that you will take the minimum deposit ($100)  from and the account amount is less than that minimum
+6. click on open new account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error: Insuffiecient amount of money found on that account, You cannot open new account using that one.
+</t>
+  </si>
+  <si>
+    <t>Account Opened!
+Congratulations, your account is now open.
+Your new account number: 16011</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify User can select and create account of Type (Checking, Saving) With message display to confirm the creation of the account. </t>
+  </si>
+  <si>
+    <t>Verify user account created with default balance ($100).</t>
+  </si>
+  <si>
+    <t>TC_USAT_003</t>
+  </si>
+  <si>
+    <t>Verify user can transfer funds to the new created account.</t>
+  </si>
+  <si>
+    <t>1. user open the website (https://parabank.parasoft.com/parabank/index.htm)
+2.Login using username &amp; password.
+3. Choose Open new account from the side menu bar.
+4. select account type from the menu (saving, checking)
+5.choose the account number that you will take the minimum deposit ($100)  from and the account amount can afford that amount.
+6. click on open new account
+7.new account will be created, click on the new account number that will appear.</t>
+  </si>
+  <si>
+    <t>1. user open the website (https://parabank.parasoft.com/parabank/index.htm)
+2.Login using username &amp; password.
+3. Choose Open new account from the side menu bar.
+4. select account type from the menu (saving, checking)
+5.choose the account number that you will take the minimum deposit ($100)  from and the account amount can afford that amount.
+6. click on open new account
+7. click on (transfer funds) from the left nav bar.
+8.choose the account you will transfer from to the new account created then write the amount above.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer done successfully.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account created successfully with the expected amount ($100)
+</t>
+  </si>
+  <si>
+    <t>TC_USAT_004</t>
+  </si>
+  <si>
+    <t>TC_USAT_005</t>
+  </si>
+  <si>
+    <t>Confirm the new account visability in the account overview.</t>
+  </si>
+  <si>
+    <t>1. user open the website (https://parabank.parasoft.com/parabank/index.htm)
+2.Login using username &amp; password.
+3. Choose Open new account from the side menu bar.
+4. select account type from the menu (saving, checking)
+5.choose the account number that you will take the minimum deposit ($100)  from and the account amount can afford that amount.
+6.click on the account overview
+7. validate the appearance of the new created account number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">account number found under the accounts overview list.
+</t>
+  </si>
+  <si>
+    <t>Verify user cannot transfer negative funds to the new created account.</t>
+  </si>
+  <si>
+    <t>1. user open the website (https://parabank.parasoft.com/parabank/index.htm)
+2.Login using username &amp; password.
+3. Choose Open new account from the side menu bar.
+4. select account type from the menu (saving, checking)
+5.choose the account number that you will take the minimum deposit ($100)  from and the account amount can afford that amount.
+6. click on open new account
+7. click on (transfer funds) from the left nav bar.
+8.choose the account you will transfer from to the new account created then write the amount above in negative.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error you cannot enter negative amount.
 </t>
   </si>
 </sst>
@@ -145,12 +246,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -199,6 +300,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -222,14 +334,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -677,8 +817,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,35 +875,178 @@
         <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H3" s="8"/>
+    <row r="3" spans="1:10" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:10" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
     <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -783,35 +1066,63 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I2">
-    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" dxfId="27" priority="45" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="26" priority="46" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="25" priority="47" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="24" priority="48" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
+  <conditionalFormatting sqref="I4">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",I4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",I4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",I4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",I5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",I5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",I5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",I5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
     <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="NOT TESTED">
-      <formula>NOT(ISERROR(SEARCH("NOT TESTED",H3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",I6)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="BLOCKED">
-      <formula>NOT(ISERROR(SEARCH("BLOCKED",H3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",I6)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",H3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FAIL",I6)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",H3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PASS",I6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3 I2" xr:uid="{08F495E9-5AFF-4D3D-AE99-1CCD918399D2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 I4:I6" xr:uid="{08F495E9-5AFF-4D3D-AE99-1CCD918399D2}">
       <formula1>"PASS, FAIL, Blocked, Not Tested"</formula1>
     </dataValidation>
   </dataValidations>
@@ -824,7 +1135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E181C81-39AE-4F69-9F16-D984F7BABC99}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Bug Report for user story 4
</commit_message>
<xml_diff>
--- a/TestCases/UserStory4.xlsx
+++ b/TestCases/UserStory4.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ParaBank\web-application-testing\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209B127F-67FA-4AD8-AFC7-89ED0399D95E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB40B87D-9A9D-427F-9827-8B27F234ED1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="869" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2445" yWindow="2760" windowWidth="21600" windowHeight="11385" tabRatio="869" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User selects account type " sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="39" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -341,91 +340,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
@@ -817,8 +732,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,58 +981,58 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I2">
-    <cfRule type="containsText" dxfId="27" priority="45" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" dxfId="15" priority="45" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="46" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="14" priority="46" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="47" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="13" priority="47" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="48" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="12" priority="48" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="8" priority="16" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",I5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",I5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",I5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="4" priority="12" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",I6)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1129,18 +1044,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E181C81-39AE-4F69-9F16-D984F7BABC99}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding api collection and report also adding presentation
</commit_message>
<xml_diff>
--- a/TestCases/UserStory4.xlsx
+++ b/TestCases/UserStory4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ParaBank\web-application-testing\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB40B87D-9A9D-427F-9827-8B27F234ED1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08982EA-A2F1-4A17-805A-0979F09DDE66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="2760" windowWidth="21600" windowHeight="11385" tabRatio="869" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="869" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User selects account type " sheetId="4" r:id="rId1"/>
@@ -732,13 +732,13 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" customWidth="1"/>
     <col min="4" max="4" width="33.42578125" customWidth="1"/>
@@ -812,7 +812,7 @@
       </c>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>

</xml_diff>